<commit_message>
Add day23 OCR run artifacts
</commit_message>
<xml_diff>
--- a/data/output/final_estimate.xlsx
+++ b/data/output/final_estimate.xlsx
@@ -999,7 +999,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="30" customWidth="1" min="1" max="1"/>
-    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="10" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1012,7 +1012,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Currency: INR</t>
+          <t>Currency: CUR</t>
         </is>
       </c>
     </row>
@@ -1035,7 +1035,7 @@
         </is>
       </c>
       <c r="B5" s="4" t="n">
-        <v>345217.5371837872</v>
+        <v>3018.75</v>
       </c>
     </row>
     <row r="6">
@@ -1045,7 +1045,7 @@
         </is>
       </c>
       <c r="B6" s="4" t="n">
-        <v>60436.6994645264</v>
+        <v>1446.5</v>
       </c>
     </row>
     <row r="7">
@@ -1055,7 +1055,7 @@
         </is>
       </c>
       <c r="B7" s="4" t="n">
-        <v>405654.2366483136</v>
+        <v>4465.25</v>
       </c>
     </row>
     <row r="8">
@@ -1065,7 +1065,7 @@
         </is>
       </c>
       <c r="B8" s="4" t="n">
-        <v>20282.71183241568</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -1075,7 +1075,7 @@
         </is>
       </c>
       <c r="B9" s="4" t="n">
-        <v>12778.10845442188</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -1085,7 +1085,7 @@
         </is>
       </c>
       <c r="B10" s="4" t="n">
-        <v>43871.50569351512</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -1095,7 +1095,7 @@
         </is>
       </c>
       <c r="B11" s="4" t="n">
-        <v>86865.58127315991</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -1105,7 +1105,7 @@
         </is>
       </c>
       <c r="B12" s="4" t="n">
-        <v>569452.1439018261</v>
+        <v>4465.25</v>
       </c>
     </row>
   </sheetData>
@@ -1160,11 +1160,7 @@
           <t>currency</t>
         </is>
       </c>
-      <c r="B4" s="3" t="inlineStr">
-        <is>
-          <t>INR</t>
-        </is>
-      </c>
+      <c r="B4" s="3" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
@@ -1172,9 +1168,7 @@
           <t>overhead_pct</t>
         </is>
       </c>
-      <c r="B5" s="3" t="n">
-        <v>5</v>
-      </c>
+      <c r="B5" s="3" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
@@ -1182,9 +1176,7 @@
           <t>contingency_pct</t>
         </is>
       </c>
-      <c r="B6" s="3" t="n">
-        <v>3</v>
-      </c>
+      <c r="B6" s="3" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
@@ -1192,9 +1184,7 @@
           <t>profit_pct</t>
         </is>
       </c>
-      <c r="B7" s="3" t="n">
-        <v>10</v>
-      </c>
+      <c r="B7" s="3" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
@@ -1202,9 +1192,7 @@
           <t>tax_pct</t>
         </is>
       </c>
-      <c r="B8" s="3" t="n">
-        <v>18</v>
-      </c>
+      <c r="B8" s="3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1226,8 +1214,8 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="17" customWidth="1" min="1" max="1"/>
-    <col width="19" customWidth="1" min="2" max="2"/>
-    <col width="18" customWidth="1" min="3" max="3"/>
+    <col width="11" customWidth="1" min="2" max="2"/>
+    <col width="10" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1266,10 +1254,10 @@
         </is>
       </c>
       <c r="B4" s="4" t="n">
-        <v>342198.7871837872</v>
+        <v>0</v>
       </c>
       <c r="C4" s="4" t="n">
-        <v>58990.1994645264</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -1669,7 +1657,7 @@
         </is>
       </c>
       <c r="B3" s="7" t="n">
-        <v>569452.1439018261</v>
+        <v>4465.25</v>
       </c>
     </row>
   </sheetData>
@@ -1728,7 +1716,7 @@
         </is>
       </c>
       <c r="B4" s="8" t="n">
-        <v>342198.7871837872</v>
+        <v>0</v>
       </c>
       <c r="C4" s="8" t="n">
         <v>3018.75</v>
@@ -1741,7 +1729,7 @@
         </is>
       </c>
       <c r="B5" s="8" t="n">
-        <v>58990.1994645264</v>
+        <v>0</v>
       </c>
       <c r="C5" s="8" t="n">
         <v>1446.5</v>
@@ -1754,7 +1742,7 @@
         </is>
       </c>
       <c r="B6" s="8" t="n">
-        <v>401188.9866483136</v>
+        <v>0</v>
       </c>
       <c r="C6" s="8" t="n">
         <v>4465.25</v>
@@ -1791,7 +1779,7 @@
         </is>
       </c>
       <c r="B10" s="8" t="n">
-        <v>342198.7871837872</v>
+        <v>0</v>
       </c>
       <c r="C10" s="8" t="n">
         <v>3018.75</v>
@@ -1804,7 +1792,7 @@
         </is>
       </c>
       <c r="B11" s="8" t="n">
-        <v>58990.1994645264</v>
+        <v>0</v>
       </c>
       <c r="C11" s="8" t="n">
         <v>1446.5</v>

</xml_diff>

<commit_message>
Day 24.1 complete: manual scale override + geometry fallback + UI updates
</commit_message>
<xml_diff>
--- a/data/output/final_estimate.xlsx
+++ b/data/output/final_estimate.xlsx
@@ -999,7 +999,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="30" customWidth="1" min="1" max="1"/>
-    <col width="10" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1012,7 +1012,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Currency: CUR</t>
+          <t>Currency: INR</t>
         </is>
       </c>
     </row>
@@ -1035,7 +1035,7 @@
         </is>
       </c>
       <c r="B5" s="4" t="n">
-        <v>3018.75</v>
+        <v>345217.5371837872</v>
       </c>
     </row>
     <row r="6">
@@ -1045,7 +1045,7 @@
         </is>
       </c>
       <c r="B6" s="4" t="n">
-        <v>1446.5</v>
+        <v>60436.6994645264</v>
       </c>
     </row>
     <row r="7">
@@ -1055,7 +1055,7 @@
         </is>
       </c>
       <c r="B7" s="4" t="n">
-        <v>4465.25</v>
+        <v>405654.2366483136</v>
       </c>
     </row>
     <row r="8">
@@ -1065,7 +1065,7 @@
         </is>
       </c>
       <c r="B8" s="4" t="n">
-        <v>0</v>
+        <v>20282.71183241568</v>
       </c>
     </row>
     <row r="9">
@@ -1075,7 +1075,7 @@
         </is>
       </c>
       <c r="B9" s="4" t="n">
-        <v>0</v>
+        <v>12778.10845442188</v>
       </c>
     </row>
     <row r="10">
@@ -1085,7 +1085,7 @@
         </is>
       </c>
       <c r="B10" s="4" t="n">
-        <v>0</v>
+        <v>43871.50569351512</v>
       </c>
     </row>
     <row r="11">
@@ -1095,7 +1095,7 @@
         </is>
       </c>
       <c r="B11" s="4" t="n">
-        <v>0</v>
+        <v>86865.58127315991</v>
       </c>
     </row>
     <row r="12">
@@ -1105,7 +1105,7 @@
         </is>
       </c>
       <c r="B12" s="4" t="n">
-        <v>4465.25</v>
+        <v>569452.1439018261</v>
       </c>
     </row>
   </sheetData>
@@ -1160,7 +1160,11 @@
           <t>currency</t>
         </is>
       </c>
-      <c r="B4" s="3" t="inlineStr"/>
+      <c r="B4" s="3" t="inlineStr">
+        <is>
+          <t>INR</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
@@ -1168,7 +1172,9 @@
           <t>overhead_pct</t>
         </is>
       </c>
-      <c r="B5" s="3" t="inlineStr"/>
+      <c r="B5" s="3" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
@@ -1176,7 +1182,9 @@
           <t>contingency_pct</t>
         </is>
       </c>
-      <c r="B6" s="3" t="inlineStr"/>
+      <c r="B6" s="3" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
@@ -1184,7 +1192,9 @@
           <t>profit_pct</t>
         </is>
       </c>
-      <c r="B7" s="3" t="inlineStr"/>
+      <c r="B7" s="3" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
@@ -1192,7 +1202,9 @@
           <t>tax_pct</t>
         </is>
       </c>
-      <c r="B8" s="3" t="inlineStr"/>
+      <c r="B8" s="3" t="n">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1214,8 +1226,8 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="17" customWidth="1" min="1" max="1"/>
-    <col width="11" customWidth="1" min="2" max="2"/>
-    <col width="10" customWidth="1" min="3" max="3"/>
+    <col width="19" customWidth="1" min="2" max="2"/>
+    <col width="18" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1254,10 +1266,10 @@
         </is>
       </c>
       <c r="B4" s="4" t="n">
-        <v>0</v>
+        <v>342198.7871837872</v>
       </c>
       <c r="C4" s="4" t="n">
-        <v>0</v>
+        <v>58990.1994645264</v>
       </c>
     </row>
     <row r="5">
@@ -1657,7 +1669,7 @@
         </is>
       </c>
       <c r="B3" s="7" t="n">
-        <v>4465.25</v>
+        <v>569452.1439018261</v>
       </c>
     </row>
   </sheetData>
@@ -1716,7 +1728,7 @@
         </is>
       </c>
       <c r="B4" s="8" t="n">
-        <v>0</v>
+        <v>342198.7871837872</v>
       </c>
       <c r="C4" s="8" t="n">
         <v>3018.75</v>
@@ -1729,7 +1741,7 @@
         </is>
       </c>
       <c r="B5" s="8" t="n">
-        <v>0</v>
+        <v>58990.1994645264</v>
       </c>
       <c r="C5" s="8" t="n">
         <v>1446.5</v>
@@ -1742,7 +1754,7 @@
         </is>
       </c>
       <c r="B6" s="8" t="n">
-        <v>0</v>
+        <v>401188.9866483136</v>
       </c>
       <c r="C6" s="8" t="n">
         <v>4465.25</v>
@@ -1779,7 +1791,7 @@
         </is>
       </c>
       <c r="B10" s="8" t="n">
-        <v>0</v>
+        <v>342198.7871837872</v>
       </c>
       <c r="C10" s="8" t="n">
         <v>3018.75</v>
@@ -1792,7 +1804,7 @@
         </is>
       </c>
       <c r="B11" s="8" t="n">
-        <v>0</v>
+        <v>58990.1994645264</v>
       </c>
       <c r="C11" s="8" t="n">
         <v>1446.5</v>

</xml_diff>